<commit_message>
Alice is the best.
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/Diving_log_Spring_2023_BenthFun.xlsx
+++ b/Data/Spring_2023/Diving_log_Spring_2023_BenthFun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/Spring_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BA7A57-FE28-744A-A394-269202D49CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B375FC77-716C-874F-AAC7-F93AA5BD6314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15980" activeTab="1" xr2:uid="{AC65A032-FAEB-0942-B0EC-C9C433D5231F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="214">
   <si>
     <t>Diving_Date</t>
   </si>
@@ -610,6 +610,72 @@
   </si>
   <si>
     <t>E6</t>
+  </si>
+  <si>
+    <t>Tn_t1_ELOW_tile_01</t>
+  </si>
+  <si>
+    <t>Tn_t1_ELOW_tile_02</t>
+  </si>
+  <si>
+    <t>Tn_t1_ELOW_tile_03</t>
+  </si>
+  <si>
+    <t>Tn_t1_ELOW_blank_01</t>
+  </si>
+  <si>
+    <t>Tn_t1_ELOW_tile_04</t>
+  </si>
+  <si>
+    <t>Tn_t1_ELOW_tile_05</t>
+  </si>
+  <si>
+    <t>Tn_t1_ELOW_tile_06</t>
+  </si>
+  <si>
+    <t>Tn_t1_ELOW_blank_02</t>
+  </si>
+  <si>
+    <t>Tn_t1_LOW_tile_01</t>
+  </si>
+  <si>
+    <t>Tn_t1_LOW_tile_02</t>
+  </si>
+  <si>
+    <t>Tn_t1_LOW_tile_03</t>
+  </si>
+  <si>
+    <t>Tn_t1_LOW_blank_01</t>
+  </si>
+  <si>
+    <t>Tn_t1_LOW_tile_04</t>
+  </si>
+  <si>
+    <t>Tn_t1_LOW_tile_05</t>
+  </si>
+  <si>
+    <t>Tn_t1_LOW_tile_06</t>
+  </si>
+  <si>
+    <t>Tn_t1_LOW_blank_02</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>L6</t>
   </si>
 </sst>
 </file>
@@ -3783,10 +3849,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8096E2FE-6459-2147-9706-235887F73F2A}">
-  <dimension ref="A1:J180"/>
+  <dimension ref="A1:J194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="K177" sqref="K177"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="J189" sqref="J189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8770,7 +8836,7 @@
         <v>45090</v>
       </c>
       <c r="B167" t="s">
-        <v>9</v>
+        <v>192</v>
       </c>
       <c r="C167" t="s">
         <v>17</v>
@@ -8802,7 +8868,7 @@
         <v>45090</v>
       </c>
       <c r="B168" t="s">
-        <v>10</v>
+        <v>193</v>
       </c>
       <c r="C168" t="s">
         <v>18</v>
@@ -8834,7 +8900,7 @@
         <v>45090</v>
       </c>
       <c r="B169" t="s">
-        <v>11</v>
+        <v>194</v>
       </c>
       <c r="C169" t="s">
         <v>19</v>
@@ -8866,7 +8932,7 @@
         <v>45090</v>
       </c>
       <c r="B170" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="C170" t="s">
         <v>20</v>
@@ -8983,7 +9049,7 @@
         <v>45090</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>12</v>
+        <v>196</v>
       </c>
       <c r="C174" t="s">
         <v>21</v>
@@ -9015,7 +9081,7 @@
         <v>45090</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>14</v>
+        <v>197</v>
       </c>
       <c r="C175" t="s">
         <v>22</v>
@@ -9047,7 +9113,7 @@
         <v>45090</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>15</v>
+        <v>198</v>
       </c>
       <c r="C176" t="s">
         <v>23</v>
@@ -9079,7 +9145,7 @@
         <v>45090</v>
       </c>
       <c r="B177" t="s">
-        <v>16</v>
+        <v>199</v>
       </c>
       <c r="C177" t="s">
         <v>24</v>
@@ -9189,6 +9255,222 @@
       </c>
       <c r="J180" s="3">
         <v>-36.4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A181" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B181" t="s">
+        <v>200</v>
+      </c>
+      <c r="C181" t="s">
+        <v>17</v>
+      </c>
+      <c r="G181">
+        <v>1</v>
+      </c>
+      <c r="H181" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B182" t="s">
+        <v>201</v>
+      </c>
+      <c r="C182" t="s">
+        <v>18</v>
+      </c>
+      <c r="G182">
+        <v>2</v>
+      </c>
+      <c r="H182" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B183" t="s">
+        <v>202</v>
+      </c>
+      <c r="C183" t="s">
+        <v>19</v>
+      </c>
+      <c r="G183">
+        <v>3</v>
+      </c>
+      <c r="H183" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B184" t="s">
+        <v>203</v>
+      </c>
+      <c r="C184" t="s">
+        <v>20</v>
+      </c>
+      <c r="G184">
+        <v>4</v>
+      </c>
+      <c r="H184" s="9"/>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A185" s="1">
+        <v>45091</v>
+      </c>
+      <c r="C185" t="s">
+        <v>25</v>
+      </c>
+      <c r="G185">
+        <v>5</v>
+      </c>
+      <c r="H185" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A186" s="1">
+        <v>45091</v>
+      </c>
+      <c r="C186" t="s">
+        <v>26</v>
+      </c>
+      <c r="G186">
+        <v>6</v>
+      </c>
+      <c r="H186" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A187" s="1">
+        <v>45091</v>
+      </c>
+      <c r="C187" t="s">
+        <v>27</v>
+      </c>
+      <c r="G187">
+        <v>7</v>
+      </c>
+      <c r="H187" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A188" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C188" t="s">
+        <v>21</v>
+      </c>
+      <c r="G188">
+        <v>5</v>
+      </c>
+      <c r="H188" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A189" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C189" t="s">
+        <v>22</v>
+      </c>
+      <c r="G189">
+        <v>6</v>
+      </c>
+      <c r="H189" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A190" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C190" t="s">
+        <v>23</v>
+      </c>
+      <c r="G190">
+        <v>7</v>
+      </c>
+      <c r="H190" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B191" t="s">
+        <v>207</v>
+      </c>
+      <c r="C191" t="s">
+        <v>24</v>
+      </c>
+      <c r="G191">
+        <v>4</v>
+      </c>
+      <c r="H191" s="9"/>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A192" s="1">
+        <v>45091</v>
+      </c>
+      <c r="C192" t="s">
+        <v>29</v>
+      </c>
+      <c r="G192">
+        <v>1</v>
+      </c>
+      <c r="H192" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A193" s="1">
+        <v>45091</v>
+      </c>
+      <c r="C193" t="s">
+        <v>30</v>
+      </c>
+      <c r="G193">
+        <v>2</v>
+      </c>
+      <c r="H193" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A194" s="1">
+        <v>45091</v>
+      </c>
+      <c r="C194" t="s">
+        <v>31</v>
+      </c>
+      <c r="G194">
+        <v>3</v>
+      </c>
+      <c r="H194" s="9" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>